<commit_message>
Commit om merge uit te kunnen voeren
</commit_message>
<xml_diff>
--- a/catalogusdata/BAG/Beslisboom Pand BAG T.xlsx
+++ b/catalogusdata/BAG/Beslisboom Pand BAG T.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="170">
   <si>
     <t>tabblad</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>rdfs</t>
-  </si>
-  <si>
-    <t>dcterms</t>
   </si>
   <si>
     <t>vocabulaire-conditie</t>
@@ -512,18 +509,6 @@
     <t>http://{source}</t>
   </si>
   <si>
-    <t xml:space="preserve">source </t>
-  </si>
-  <si>
-    <t>Bron</t>
-  </si>
-  <si>
-    <t>wetten.overheid.nl/jci1.3:c:BWBR0023466</t>
-  </si>
-  <si>
-    <t>zoek.officielebekendmakingen.nl/kst-30968-3.html</t>
-  </si>
-  <si>
     <t>www.parlementairemonitor.nl/9353000/1/j9vvij5epmj1ey0/vk57jvazlov8</t>
   </si>
   <si>
@@ -582,6 +567,15 @@
   </si>
   <si>
     <t>http://data.test.pdok.nl/catalogus/bag/id/concept/{toeleidingsbegrip}</t>
+  </si>
+  <si>
+    <t>dct</t>
+  </si>
+  <si>
+    <t>&lt;wetten.overheid.nl/jci1.3:c:BWBR0023466&gt;</t>
+  </si>
+  <si>
+    <t>&lt;zoek.officielebekendmakingen.nl/kst-30968-3.html&gt;</t>
   </si>
 </sst>
 </file>
@@ -648,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -660,18 +654,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -980,7 +965,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1045,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -1062,13 +1047,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,10 +1064,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,10 +1092,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,300 +1106,300 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="B27" t="s">
-        <v>83</v>
-      </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,42 +1458,41 @@
     <hyperlink ref="D2" r:id="rId4" location="{klasse}"/>
     <hyperlink ref="D9" r:id="rId5" location="{eigenschap}"/>
     <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D23" r:id="rId7"/>
-    <hyperlink ref="D13" r:id="rId8" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
-    <hyperlink ref="D14" r:id="rId9" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
-    <hyperlink ref="D15" r:id="rId10" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
-    <hyperlink ref="D16" r:id="rId11" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
-    <hyperlink ref="D17" r:id="rId12" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
-    <hyperlink ref="D10" r:id="rId13" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D12" r:id="rId14" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D11" r:id="rId15" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
-    <hyperlink ref="D18" r:id="rId16" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{focus}"/>
-    <hyperlink ref="D19" r:id="rId17" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{hetzelfde}"/>
-    <hyperlink ref="D20" r:id="rId18" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{gerelateerd}"/>
-    <hyperlink ref="D21" r:id="rId19" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{brederdan}"/>
-    <hyperlink ref="D22" r:id="rId20" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{engerdan}"/>
-    <hyperlink ref="D24" r:id="rId21" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D25" r:id="rId22" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D30" r:id="rId23"/>
-    <hyperlink ref="D29" r:id="rId24" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D27" r:id="rId25" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
-    <hyperlink ref="D28" r:id="rId26" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D33" r:id="rId27" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{toeleidingsbegrip}"/>
-    <hyperlink ref="D34" r:id="rId28" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D26" r:id="rId29" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
-    <hyperlink ref="D31" r:id="rId30" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
+    <hyperlink ref="D13" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
+    <hyperlink ref="D14" r:id="rId8" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
+    <hyperlink ref="D15" r:id="rId9" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
+    <hyperlink ref="D16" r:id="rId10" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
+    <hyperlink ref="D17" r:id="rId11" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
+    <hyperlink ref="D10" r:id="rId12" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D11" r:id="rId13" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
+    <hyperlink ref="D18" r:id="rId14" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{focus}"/>
+    <hyperlink ref="D19" r:id="rId15" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{hetzelfde}"/>
+    <hyperlink ref="D20" r:id="rId16" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{gerelateerd}"/>
+    <hyperlink ref="D21" r:id="rId17" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{brederdan}"/>
+    <hyperlink ref="D22" r:id="rId18" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{engerdan}"/>
+    <hyperlink ref="D23" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D30" r:id="rId21"/>
+    <hyperlink ref="D29" r:id="rId22"/>
+    <hyperlink ref="D27" r:id="rId23" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
+    <hyperlink ref="D28" r:id="rId24" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D33" r:id="rId25" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{toeleidingsbegrip}"/>
+    <hyperlink ref="D34" r:id="rId26" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D26" r:id="rId27" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
+    <hyperlink ref="D31" r:id="rId28" display="http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}"/>
+    <hyperlink ref="D12" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,627 +1525,617 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>74</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="D33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="D34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-    </row>
-    <row r="56" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
@@ -2169,13 +2143,6 @@
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2185,10 +2152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,555 +2176,575 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="3" t="s">
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2"/>
-      <c r="I2" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="J2"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2"/>
       <c r="O2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2"/>
+    </row>
+    <row r="3" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="3"/>
+      <c r="G3"/>
       <c r="H3"/>
-      <c r="I3" s="2" t="s">
-        <v>142</v>
+      <c r="I3" t="s">
+        <v>141</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3"/>
       <c r="O3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P3"/>
     </row>
-    <row r="4" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>117</v>
+    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
       </c>
       <c r="C4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>133</v>
+      <c r="D4"/>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
       <c r="M4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>117</v>
+      <c r="N4"/>
+      <c r="O4" t="s">
+        <v>100</v>
+      </c>
+      <c r="P4"/>
+    </row>
+    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>133</v>
+      <c r="D5"/>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
       <c r="M5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>118</v>
+      <c r="N5"/>
+      <c r="O5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
       </c>
       <c r="C6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>134</v>
+      <c r="D6"/>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" t="s">
+        <v>133</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
-      <c r="I6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="I6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
       <c r="M6"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>118</v>
+      <c r="N6"/>
+      <c r="O6" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
       </c>
       <c r="C7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>134</v>
+      <c r="D7"/>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
+        <v>133</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="I7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>119</v>
+      <c r="N7"/>
+      <c r="O7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
       </c>
       <c r="C8"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>135</v>
+      <c r="D8"/>
+      <c r="E8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" t="s">
+        <v>134</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
-      <c r="I8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="I8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
       <c r="M8"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="N8"/>
+      <c r="O8" t="s">
         <v>119</v>
       </c>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
       <c r="C9"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>135</v>
+      <c r="D9"/>
+      <c r="E9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" t="s">
+        <v>134</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
-      <c r="I9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
       <c r="M9"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="9" t="s">
+      <c r="N9"/>
+      <c r="O9" t="s">
+        <v>120</v>
+      </c>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="C10"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>136</v>
+      <c r="D10"/>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" t="s">
+        <v>135</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
-      <c r="I10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="I10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
       <c r="M10"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="N10"/>
+      <c r="O10" t="s">
         <v>122</v>
       </c>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
       <c r="C11"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>136</v>
+      <c r="D11"/>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
-      <c r="I11" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="I11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
       <c r="M11"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>122</v>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
       </c>
       <c r="C12"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>136</v>
+      <c r="D12"/>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
-      <c r="I12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="I12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
       <c r="M12"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>124</v>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
       </c>
       <c r="C13"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>137</v>
+      <c r="D13"/>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" t="s">
+        <v>136</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
-      <c r="I13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="I13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="N13"/>
+      <c r="O13" t="s">
         <v>124</v>
       </c>
+      <c r="P13"/>
+    </row>
+    <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
       <c r="C14"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>137</v>
+      <c r="D14"/>
+      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" t="s">
+        <v>136</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
-      <c r="I14" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="I14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>124</v>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+    </row>
+    <row r="15" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
       </c>
       <c r="C15"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>137</v>
+      <c r="D15"/>
+      <c r="E15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" t="s">
+        <v>136</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
-      <c r="I15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="I15" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>111</v>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+    </row>
+    <row r="16" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>138</v>
+      <c r="D16"/>
+      <c r="E16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" t="s">
+        <v>137</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="I16" s="2" t="s">
-        <v>141</v>
+      <c r="I16" t="s">
+        <v>140</v>
       </c>
       <c r="J16"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16"/>
+      <c r="L16"/>
       <c r="M16"/>
-      <c r="N16" s="5"/>
+      <c r="N16"/>
       <c r="O16"/>
-    </row>
-    <row r="17" spans="1:22" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>111</v>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>138</v>
+      <c r="D17"/>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" t="s">
+        <v>137</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
-      <c r="I17" s="2" t="s">
-        <v>142</v>
+      <c r="I17" t="s">
+        <v>141</v>
       </c>
       <c r="J17"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17"/>
+      <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="5"/>
+      <c r="N17"/>
       <c r="O17"/>
-    </row>
-    <row r="18" spans="1:22" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>112</v>
+      <c r="P17"/>
+    </row>
+    <row r="18" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="D18"/>
+      <c r="E18" t="s">
         <v>139</v>
+      </c>
+      <c r="F18" t="s">
+        <v>138</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
-      <c r="I18" s="2" t="s">
-        <v>141</v>
+      <c r="I18" t="s">
+        <v>140</v>
       </c>
       <c r="J18"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="K18"/>
+      <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="5"/>
+      <c r="N18"/>
       <c r="O18"/>
-    </row>
-    <row r="19" spans="1:22" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>112</v>
+      <c r="P18"/>
+    </row>
+    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" s="14" t="s">
+      <c r="D19"/>
+      <c r="E19" t="s">
         <v>139</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
-      <c r="I19" s="2" t="s">
-        <v>142</v>
+      <c r="I19" t="s">
+        <v>141</v>
       </c>
       <c r="J19"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="K19"/>
+      <c r="L19"/>
       <c r="M19"/>
-      <c r="N19" s="5"/>
+      <c r="N19"/>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
@@ -2770,7 +2757,7 @@
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -2803,24 +2790,9 @@
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="3"/>
-    </row>
-    <row r="46" spans="6:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="6:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="6:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="http://wetten.overheid.nl/jci1.3:c:BWBR0023466"/>
@@ -2852,7 +2824,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,180 +2836,180 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="390" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <v>42933</v>
+      </c>
+      <c r="H2" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="10">
-        <v>42933</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="10">
+        <v>112</v>
+      </c>
+      <c r="G3">
         <v>42933</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="10">
+        <v>112</v>
+      </c>
+      <c r="G4">
         <v>42933</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="10">
+        <v>112</v>
+      </c>
+      <c r="G5">
         <v>42933</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="10">
+        <v>112</v>
+      </c>
+      <c r="G6">
         <v>42933</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="10">
+        <v>112</v>
+      </c>
+      <c r="G7">
         <v>42933</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" s="10">
+        <v>112</v>
+      </c>
+      <c r="G8">
         <v>42933</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="10">
+        <v>112</v>
+      </c>
+      <c r="G9">
         <v>42933</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="10"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="10"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G12" s="10"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="10"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="10"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="10"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="10"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="10"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="10"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="10"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="10"/>
+      <c r="G20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3061,44 +3033,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="10"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="10"/>
+      <c r="C12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3108,120 +3080,139 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>141</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>128</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>142</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
         <v>129</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>143</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
         <v>130</v>
       </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>144</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
         <v>131</v>
       </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>154</v>
+      <c r="F6" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3231,11 +3222,11 @@
     <hyperlink ref="A4" r:id="rId3" display="https://www.parlementairemonitor.nl/9353000/1/j9vvij5epmj1ey0/vk57jvazlov8"/>
     <hyperlink ref="A5" r:id="rId4" display="https://www.nen.nl/NEN-Shop/Norm/NEN-25802007-nl.htm"/>
     <hyperlink ref="A6" r:id="rId5" display="https://zoek.officielebekendmakingen.nl/kst-31726-7.html"/>
-    <hyperlink ref="E2" r:id="rId6" display="http://wetten.overheid.nl/jci1.3:c:BWBR0023466"/>
-    <hyperlink ref="E3" r:id="rId7" display="https://zoek.officielebekendmakingen.nl/kst-30968-3.html"/>
-    <hyperlink ref="E4" r:id="rId8"/>
-    <hyperlink ref="E5" r:id="rId9"/>
-    <hyperlink ref="E6" r:id="rId10" display="https://zoek.officielebekendmakingen.nl/kst-31726-7.html"/>
+    <hyperlink ref="F2" r:id="rId6" display="http://wetten.overheid.nl/jci1.3:c:BWBR0023466"/>
+    <hyperlink ref="F3" r:id="rId7" display="https://zoek.officielebekendmakingen.nl/kst-30968-3.html"/>
+    <hyperlink ref="F4" r:id="rId8"/>
+    <hyperlink ref="F5" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10" display="https://zoek.officielebekendmakingen.nl/kst-31726-7.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>